<commit_message>
Complete data cleaning and development of NMA functions
</commit_message>
<xml_diff>
--- a/data_from_lab/rop_codebook.xlsx
+++ b/data_from_lab/rop_codebook.xlsx
@@ -15,6 +15,7 @@
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
     <sheet name="variable types" sheetId="3" r:id="rId2"/>
     <sheet name="missing_data" sheetId="4" r:id="rId3"/>
+    <sheet name="intervention codes" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="203">
   <si>
     <t>code</t>
   </si>
@@ -212,18 +213,6 @@
     <t>third comparator</t>
   </si>
   <si>
-    <t>what class of intervention in control</t>
-  </si>
-  <si>
-    <t>what class of intervention in treatment 1</t>
-  </si>
-  <si>
-    <t>what class of intervention in treatment 2</t>
-  </si>
-  <si>
-    <t>what class of intervention in treatment 3</t>
-  </si>
-  <si>
     <t>what was the method of eye assessment</t>
   </si>
   <si>
@@ -516,13 +505,145 @@
   </si>
   <si>
     <t>anynotes</t>
+  </si>
+  <si>
+    <t>intervention_name</t>
+  </si>
+  <si>
+    <t>class_code</t>
+  </si>
+  <si>
+    <t>drops</t>
+  </si>
+  <si>
+    <t>drops.nospec</t>
+  </si>
+  <si>
+    <t>drops.ss</t>
+  </si>
+  <si>
+    <t>drops no spec</t>
+  </si>
+  <si>
+    <t>drops sweet mult</t>
+  </si>
+  <si>
+    <t>drops.sweet</t>
+  </si>
+  <si>
+    <t>drops sweet</t>
+  </si>
+  <si>
+    <t>drops.wfdri</t>
+  </si>
+  <si>
+    <t>drops wfdri</t>
+  </si>
+  <si>
+    <t>ebm.drops</t>
+  </si>
+  <si>
+    <t>drops ebm mult</t>
+  </si>
+  <si>
+    <t>feed.1hr.drops</t>
+  </si>
+  <si>
+    <t>drops diet 1hr</t>
+  </si>
+  <si>
+    <t>feed.2hr.drops</t>
+  </si>
+  <si>
+    <t>drops diet 2hr</t>
+  </si>
+  <si>
+    <t>morphine.drops</t>
+  </si>
+  <si>
+    <t>drops morph</t>
+  </si>
+  <si>
+    <t>NIDCAP</t>
+  </si>
+  <si>
+    <t>nns.drops</t>
+  </si>
+  <si>
+    <t>drops phys</t>
+  </si>
+  <si>
+    <t>nns.ebm.drops</t>
+  </si>
+  <si>
+    <t>nns.sweet.drops</t>
+  </si>
+  <si>
+    <t>N2O.sweet.drops</t>
+  </si>
+  <si>
+    <t>drops.N2O.sweet</t>
+  </si>
+  <si>
+    <t>nns</t>
+  </si>
+  <si>
+    <t>phys</t>
+  </si>
+  <si>
+    <t>no.treatment</t>
+  </si>
+  <si>
+    <t>placebo</t>
+  </si>
+  <si>
+    <t>acetaminophen.drops</t>
+  </si>
+  <si>
+    <t>drops.acet</t>
+  </si>
+  <si>
+    <t>sensorial.sat</t>
+  </si>
+  <si>
+    <t>sweet</t>
+  </si>
+  <si>
+    <t>sweet.drops</t>
+  </si>
+  <si>
+    <t>sweet.nns.drops</t>
+  </si>
+  <si>
+    <t>sweet.rep</t>
+  </si>
+  <si>
+    <t>sweet.sing</t>
+  </si>
+  <si>
+    <t>sweet sing</t>
+  </si>
+  <si>
+    <t>sweet rep</t>
+  </si>
+  <si>
+    <t>WFDRI.drops</t>
+  </si>
+  <si>
+    <t>drops WFDRI</t>
+  </si>
+  <si>
+    <t>scaled_score</t>
+  </si>
+  <si>
+    <t>was the score scaled?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,16 +677,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -573,11 +707,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -588,6 +733,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -931,16 +1080,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,10 +1100,10 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,10 +1114,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,10 +1128,10 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,10 +1142,10 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,10 +1156,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,10 +1170,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,10 +1184,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,10 +1198,10 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1063,10 +1212,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,10 +1226,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,10 +1240,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,10 +1254,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1119,10 +1268,10 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,10 +1282,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,10 +1296,10 @@
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,10 +1310,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1175,10 +1324,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,10 +1338,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,10 +1352,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1217,10 +1366,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1231,10 +1380,10 @@
         <v>17</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,10 +1394,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,10 +1408,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,10 +1422,10 @@
         <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,10 +1436,10 @@
         <v>17</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,24 +1450,24 @@
         <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1329,24 +1478,24 @@
         <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,24 +1506,24 @@
         <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1385,24 +1534,24 @@
         <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1413,24 +1562,24 @@
         <v>17</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1441,24 +1590,24 @@
         <v>17</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1469,24 +1618,24 @@
         <v>17</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1497,10 +1646,10 @@
         <v>17</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,10 +1660,10 @@
         <v>17</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,10 +1674,10 @@
         <v>17</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1539,10 +1688,10 @@
         <v>17</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1553,10 +1702,10 @@
         <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1567,38 +1716,38 @@
         <v>17</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,391 +1755,391 @@
         <v>7</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2006,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF0C585-0929-4EA4-B93B-123192197F29}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2185,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>48</v>
@@ -2218,7 +2367,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>61</v>
@@ -2232,7 +2381,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>62</v>
@@ -2246,7 +2395,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>63</v>
@@ -2260,7 +2409,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>64</v>
@@ -2274,7 +2423,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>65</v>
@@ -2288,7 +2437,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>66</v>
@@ -2297,12 +2446,12 @@
         <v>17</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>67</v>
@@ -2311,12 +2460,12 @@
         <v>17</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>68</v>
@@ -2325,12 +2474,12 @@
         <v>17</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>69</v>
@@ -2344,7 +2493,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>70</v>
@@ -2353,43 +2502,43 @@
         <v>17</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>17</v>
@@ -2400,10 +2549,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>17</v>
@@ -2414,24 +2563,24 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>17</v>
@@ -2442,24 +2591,24 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>17</v>
@@ -2470,10 +2619,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>17</v>
@@ -2484,10 +2633,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>17</v>
@@ -2498,7 +2647,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>95</v>
@@ -2512,10 +2661,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>17</v>
@@ -2540,10 +2689,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>17</v>
@@ -2554,10 +2703,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>17</v>
@@ -2568,10 +2717,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>17</v>
@@ -2582,10 +2731,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>17</v>
@@ -2596,7 +2745,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>81</v>
@@ -2610,7 +2759,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>82</v>
@@ -2624,97 +2773,97 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>44</v>
+      <c r="A45" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>15</v>
+        <v>112</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>45</v>
+      <c r="A46" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>46</v>
+      <c r="A47" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>15</v>
+        <v>114</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>87</v>
+      <c r="A48" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>15</v>
+        <v>115</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>88</v>
+      <c r="A49" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>116</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>7</v>
+      <c r="A50" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>4</v>
@@ -2722,13 +2871,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>4</v>
@@ -2736,55 +2885,55 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>4</v>
@@ -2792,13 +2941,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>5</v>
@@ -2806,13 +2955,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>5</v>
@@ -2820,13 +2969,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>146</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>5</v>
@@ -2834,27 +2983,27 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>5</v>
@@ -2862,13 +3011,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>5</v>
@@ -2876,13 +3025,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>5</v>
@@ -2890,13 +3039,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>5</v>
@@ -2910,7 +3059,7 @@
         <v>151</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>5</v>
@@ -2924,7 +3073,7 @@
         <v>152</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>5</v>
@@ -2938,7 +3087,7 @@
         <v>153</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>5</v>
@@ -2952,7 +3101,7 @@
         <v>154</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>5</v>
@@ -2966,7 +3115,7 @@
         <v>155</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>5</v>
@@ -2977,10 +3126,10 @@
         <v>137</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>5</v>
@@ -2991,10 +3140,10 @@
         <v>138</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>5</v>
@@ -3005,10 +3154,10 @@
         <v>139</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>5</v>
@@ -3019,13 +3168,13 @@
         <v>140</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3033,10 +3182,10 @@
         <v>141</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>5</v>
@@ -3044,72 +3193,30 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>115</v>
+        <v>158</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>15</v>
+      <c r="A75" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3132,32 +3239,251 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F1E402-9E58-46F7-B4FF-74E444A5BF74}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>